<commit_message>
changed the dataframe locator from index-based to combined index-label + string
</commit_message>
<xml_diff>
--- a/input_copy_processed.xlsx
+++ b/input_copy_processed.xlsx
@@ -896,7 +896,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -972,7 +972,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1048,7 +1048,7 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1202,7 +1202,7 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1278,7 +1278,7 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1354,7 +1354,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>6.95</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1886,14 +1886,10 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>4.74</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.73</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1962,14 +1958,10 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>4.60</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.58</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -2038,14 +2030,10 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>4.89</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.14 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2114,14 +2102,10 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>4.89</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.14 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
@@ -2190,14 +2174,10 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>4.89</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.14 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2266,14 +2246,10 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4.89</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>5:3,10:6,20:9,30:12,40:15</t>
-        </is>
-      </c>
+          <t>4.14 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -2342,14 +2318,10 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>21.39</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>3:3,6:6,9:9,12:12,15:15</t>
-        </is>
-      </c>
+          <t>18.04 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -2418,14 +2390,10 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>21.39</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>3:3,6:6,9:9,12:12,15:15</t>
-        </is>
-      </c>
+          <t>18.04 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2494,14 +2462,10 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>21.39</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>3:3,6:6,9:9,12:12,15:15</t>
-        </is>
-      </c>
+          <t>18.04 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2570,14 +2534,10 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>21.39</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>3:3,6:6,9:9,12:12,15:15</t>
-        </is>
-      </c>
+          <t>18.04 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
@@ -2646,14 +2606,10 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>21.39</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>3:3,6:6,9:9,12:12,15:15</t>
-        </is>
-      </c>
+          <t>18.04 (15.25%)</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>

</xml_diff>

<commit_message>
IMPLEMENT newly created function for extracting sales and regular price
</commit_message>
<xml_diff>
--- a/input_copy_processed.xlsx
+++ b/input_copy_processed.xlsx
@@ -1886,10 +1886,14 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>4.73</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1958,10 +1962,14 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>4.58</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -2030,10 +2038,14 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>4.14 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2102,10 +2114,14 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>4.14 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
@@ -2174,10 +2190,14 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>4.14 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2246,10 +2266,14 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4.14 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>5:3,10:6,20:9,30:12,40:15</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -2318,10 +2342,14 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>18.04 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
+          <t>21.29</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,48:15</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -2390,10 +2418,14 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>18.04 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+          <t>21.29</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,48:15</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2462,10 +2494,14 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>18.04 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+          <t>21.29</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,48:15</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2534,10 +2570,14 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>18.04 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
+          <t>21.29</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,48:15</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
@@ -2606,10 +2646,14 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>18.04 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr"/>
+          <t>21.29</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,48:15</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
@@ -2678,10 +2722,14 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>18.21 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr"/>
+          <t>21.49</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,40:15</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
@@ -2750,10 +2798,14 @@
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
-          <t>18.21 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr"/>
+          <t>21.49</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,40:15</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
@@ -2822,10 +2874,14 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr">
         <is>
-          <t>18.21 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr"/>
+          <t>21.49</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,40:15</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
@@ -2894,10 +2950,14 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>18.21 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr"/>
+          <t>21.49</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,40:15</t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
@@ -2966,10 +3026,14 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>18.21 (15.25%)</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr"/>
+          <t>21.49</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>6:3,12:6,24:9,26:12,40:15</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
@@ -3021,7 +3085,11 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>13.49</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
           <t>9.95</t>

</xml_diff>